<commit_message>
changed GCs and a few bits
</commit_message>
<xml_diff>
--- a/GCs.xlsx
+++ b/GCs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/att22_ic_ac_uk/Documents/AAYEAR4/APO1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natur\Documents\AOBaddies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="855" documentId="8_{1BB338DD-5CE3-4F3B-820B-FA7D83DA8823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4105E4B2-48B9-49C0-9732-F232B0B75AA4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD5CF5-EB09-40CD-A08F-45EA97C83165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11688" yWindow="12852" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{8EFD0542-B832-47AD-A0F7-47D90D0B881B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{8EFD0542-B832-47AD-A0F7-47D90D0B881B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="CpGC" sheetId="5" r:id="rId8"/>
     <sheet name="Chec king" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="337">
   <si>
     <t>Group</t>
   </si>
@@ -2916,6 +2916,9 @@
   </si>
   <si>
     <t>RED</t>
+  </si>
+  <si>
+    <t>ai</t>
   </si>
 </sst>
 </file>
@@ -3108,7 +3111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3149,6 +3152,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -12511,7 +12517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297960EB-DBC8-44A4-9F73-359D156C6248}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
+    <sheetView zoomScale="71" workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
@@ -15386,10 +15392,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F6FF9F-8B9B-488C-B485-3ABBC4416DFF}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15401,7 +15407,7 @@
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -15426,8 +15432,11 @@
       <c r="H1" s="13" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="20" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -15456,8 +15465,11 @@
         <f>0.0000000967</f>
         <v>9.6699999999999999E-8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -15486,8 +15498,11 @@
         <f>0.0000000119</f>
         <v>1.1900000000000001E-8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>295</v>
       </c>
@@ -15516,8 +15531,11 @@
         <f>0.00000012</f>
         <v>1.1999999999999999E-7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>296</v>
       </c>
@@ -15546,8 +15564,11 @@
         <f>0.000000301</f>
         <v>3.0100000000000001E-7</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>297</v>
       </c>
@@ -15576,8 +15597,11 @@
         <f>-0.000000103</f>
         <v>-1.03E-7</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>298</v>
       </c>
@@ -15605,8 +15629,11 @@
         <f>0.0000000356</f>
         <v>3.5600000000000001E-8</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>299</v>
       </c>
@@ -15635,8 +15662,11 @@
         <f>0.000000146</f>
         <v>1.4600000000000001E-7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>300</v>
       </c>
@@ -15665,8 +15695,11 @@
         <f>-0.0000000502</f>
         <v>-5.02E-8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>301</v>
       </c>
@@ -15694,8 +15727,11 @@
         <f>-0.000000018</f>
         <v>-1.7999999999999999E-8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>302</v>
       </c>
@@ -15724,8 +15760,11 @@
         <f>0.0000000624</f>
         <v>6.2400000000000003E-8</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>303</v>
       </c>
@@ -15754,8 +15793,11 @@
         <f>0.000000469</f>
         <v>4.6899999999999998E-7</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>304</v>
       </c>
@@ -15784,8 +15826,11 @@
         <f>-0.0000000159</f>
         <v>-1.59E-8</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>305</v>
       </c>
@@ -15814,8 +15859,11 @@
         <f>0.0000000678</f>
         <v>6.7799999999999998E-8</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>306</v>
       </c>
@@ -15843,8 +15891,11 @@
         <f>-0.0000000745</f>
         <v>-7.4499999999999999E-8</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>307</v>
       </c>
@@ -15873,8 +15924,11 @@
         <f>-0.0000000988</f>
         <v>-9.8799999999999998E-8</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>308</v>
       </c>
@@ -15903,8 +15957,11 @@
         <f>0.0000000494</f>
         <v>4.9399999999999999E-8</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>309</v>
       </c>
@@ -15933,8 +15990,11 @@
         <f>-0.0000000548</f>
         <v>-5.4800000000000001E-8</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>310</v>
       </c>
@@ -15963,8 +16023,11 @@
         <f>-0.0000000386</f>
         <v>-3.8600000000000002E-8</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>311</v>
       </c>
@@ -15992,8 +16055,11 @@
         <f>0.00000000286</f>
         <v>2.86E-9</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>312</v>
       </c>
@@ -16022,8 +16088,11 @@
         <f>-0.000000013</f>
         <v>-1.3000000000000001E-8</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>313</v>
       </c>
@@ -16052,8 +16121,11 @@
         <f>-0.0000000988</f>
         <v>-9.8799999999999998E-8</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -16082,8 +16154,11 @@
         <f>-0.0000000687</f>
         <v>-6.87E-8</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>314</v>
       </c>
@@ -16112,8 +16187,11 @@
         <f>-0.0000000452</f>
         <v>-4.5200000000000001E-8</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>315</v>
       </c>
@@ -16142,8 +16220,11 @@
         <f>-0.0000000178</f>
         <v>-1.7800000000000001E-8</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>316</v>
       </c>
@@ -16172,8 +16253,11 @@
         <f>-0.0000000976</f>
         <v>-9.76E-8</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -16201,8 +16285,11 @@
         <f>0.0000000105</f>
         <v>1.05E-8</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>317</v>
       </c>
@@ -16231,8 +16318,11 @@
         <f>-0.0000000628</f>
         <v>-6.2800000000000006E-8</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>318</v>
       </c>
@@ -16261,8 +16351,11 @@
         <f>0.000000146</f>
         <v>1.4600000000000001E-7</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>319</v>
       </c>
@@ -16287,8 +16380,11 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>320</v>
       </c>
@@ -16317,8 +16413,11 @@
         <f>-0.000000026</f>
         <v>-2.6000000000000001E-8</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>321</v>
       </c>
@@ -16347,8 +16446,11 @@
         <f>-0.0000000888</f>
         <v>-8.8800000000000001E-8</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>322</v>
       </c>
@@ -16377,8 +16479,11 @@
         <f>-0.0000000888</f>
         <v>-8.8800000000000001E-8</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>323</v>
       </c>
@@ -16406,6 +16511,9 @@
       <c r="H34">
         <f>-0.0000000211</f>
         <v>-2.11E-8</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the excel w nimin and nimax
</commit_message>
<xml_diff>
--- a/GCs.xlsx
+++ b/GCs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/att22_ic_ac_uk/Documents/AAYEAR4/APO1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="855" documentId="8_{1BB338DD-5CE3-4F3B-820B-FA7D83DA8823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4105E4B2-48B9-49C0-9732-F232B0B75AA4}"/>
+  <xr:revisionPtr revIDLastSave="911" documentId="8_{1BB338DD-5CE3-4F3B-820B-FA7D83DA8823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4AA674E-550E-4557-9964-5AFB455E8856}"/>
   <bookViews>
-    <workbookView xWindow="-11688" yWindow="12852" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{8EFD0542-B832-47AD-A0F7-47D90D0B881B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{8EFD0542-B832-47AD-A0F7-47D90D0B881B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="CpGC" sheetId="5" r:id="rId8"/>
     <sheet name="Chec king" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="338">
   <si>
     <t>Group</t>
   </si>
@@ -2903,9 +2903,6 @@
     <t>D0i</t>
   </si>
   <si>
-    <t>maxgroups</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
@@ -2916,6 +2913,15 @@
   </si>
   <si>
     <t>RED</t>
+  </si>
+  <si>
+    <t>nimax</t>
+  </si>
+  <si>
+    <t>nimin</t>
+  </si>
+  <si>
+    <t>ai</t>
   </si>
 </sst>
 </file>
@@ -3108,7 +3114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3149,6 +3155,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -12509,10 +12518,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297960EB-DBC8-44A4-9F73-359D156C6248}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView zoomScale="71" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12520,7 +12529,7 @@
     <col min="4" max="4" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>227</v>
       </c>
@@ -12554,8 +12563,14 @@
       <c r="K1" s="13" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12589,8 +12604,14 @@
       <c r="K2">
         <v>2.3800000000000002E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12624,8 +12645,14 @@
       <c r="K3">
         <v>1.66E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12659,8 +12686,14 @@
       <c r="K4">
         <v>8.3999999999999995E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12694,8 +12727,14 @@
       <c r="K5">
         <v>-1.5E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -12729,8 +12768,14 @@
       <c r="K6">
         <v>1.2E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>19</v>
       </c>
@@ -12764,8 +12809,14 @@
       <c r="K7">
         <v>5.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>8</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20</v>
       </c>
@@ -12799,8 +12850,14 @@
       <c r="K8">
         <v>3.0200000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>29</v>
       </c>
@@ -12834,8 +12891,14 @@
       <c r="K9">
         <v>4.1999999999999997E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>49</v>
       </c>
@@ -12869,8 +12932,14 @@
       <c r="K10">
         <v>2.81E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>50</v>
       </c>
@@ -12904,8 +12973,14 @@
       <c r="K11">
         <v>2.2800000000000001E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>54</v>
       </c>
@@ -12939,8 +13014,14 @@
       <c r="K12">
         <v>2.6200000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -12974,8 +13055,14 @@
       <c r="K13">
         <v>2.1399999999999999E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>57</v>
       </c>
@@ -13009,8 +13096,14 @@
       <c r="K14">
         <v>2.7900000000000001E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>58</v>
       </c>
@@ -13044,8 +13137,14 @@
       <c r="K15">
         <v>2.46E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>8</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>59</v>
       </c>
@@ -13079,8 +13178,14 @@
       <c r="K16">
         <v>1.8200000000000001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>60</v>
       </c>
@@ -13114,8 +13219,14 @@
       <c r="K17">
         <v>2.6499999999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>61</v>
       </c>
@@ -13149,8 +13260,14 @@
       <c r="K18">
         <v>1.9E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>8</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>65</v>
       </c>
@@ -13184,8 +13301,14 @@
       <c r="K19">
         <v>9.5999999999999992E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>134</v>
       </c>
@@ -13219,8 +13342,14 @@
       <c r="K20">
         <v>4.1700000000000001E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>8</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>168</v>
       </c>
@@ -13254,8 +13383,14 @@
       <c r="K21">
         <v>1.6E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>8</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>169</v>
       </c>
@@ -13289,8 +13424,14 @@
       <c r="K22">
         <v>5.8999999999999999E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>8</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>175</v>
       </c>
@@ -13324,8 +13465,14 @@
       <c r="K23">
         <v>3.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>8</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>176</v>
       </c>
@@ -13359,8 +13506,14 @@
       <c r="K24">
         <v>1.6999999999999999E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>8</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>179</v>
       </c>
@@ -13394,8 +13547,14 @@
       <c r="K25">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>8</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>180</v>
       </c>
@@ -13429,8 +13588,14 @@
       <c r="K26">
         <v>1.2E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>8</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>184</v>
       </c>
@@ -13464,8 +13629,14 @@
       <c r="K27">
         <v>1.04E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>8</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>21</v>
       </c>
@@ -13499,8 +13670,14 @@
       <c r="K28" s="14">
         <v>2.29E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>8</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>30</v>
       </c>
@@ -13534,8 +13711,14 @@
       <c r="K29" s="14">
         <v>1.7000000000000001E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>8</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>31</v>
       </c>
@@ -13569,8 +13752,14 @@
       <c r="K30" s="14">
         <v>2.07E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>8</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>32</v>
       </c>
@@ -13604,8 +13793,14 @@
       <c r="K31" s="14">
         <v>4.7800000000000002E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>8</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>62</v>
       </c>
@@ -13639,8 +13834,14 @@
       <c r="K32" s="14">
         <v>2.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>8</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>63</v>
       </c>
@@ -13674,8 +13875,14 @@
       <c r="K33" s="14">
         <v>1.18E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>8</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>126</v>
       </c>
@@ -13709,8 +13916,14 @@
       <c r="K34" s="14">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>8</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>128</v>
       </c>
@@ -13744,8 +13957,14 @@
       <c r="K35" s="14">
         <v>2.1299999999999999E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>148</v>
       </c>
@@ -13779,8 +13998,14 @@
       <c r="K36" s="14">
         <v>1.43E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>8</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>149</v>
       </c>
@@ -13814,8 +14039,14 @@
       <c r="K37" s="14">
         <v>2.3699999999999999E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <v>8</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>170</v>
       </c>
@@ -13848,6 +14079,12 @@
       </c>
       <c r="K38" s="14">
         <v>0.13930000000000001</v>
+      </c>
+      <c r="L38">
+        <v>8</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -15064,10 +15301,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7EBF146-937E-4601-B58E-56AADBC56C60}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15075,308 +15312,533 @@
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>291</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="C1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>237</v>
       </c>
       <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>239</v>
       </c>
       <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>247</v>
       </c>
       <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
       <c r="B9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>257</v>
       </c>
       <c r="B10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>258</v>
       </c>
       <c r="B11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>259</v>
       </c>
       <c r="B12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>260</v>
       </c>
       <c r="B13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>261</v>
       </c>
       <c r="B14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>262</v>
       </c>
       <c r="B15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
       <c r="B16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>263</v>
       </c>
       <c r="B17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>264</v>
       </c>
       <c r="B18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>266</v>
       </c>
       <c r="B19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>278</v>
       </c>
       <c r="B20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>288</v>
       </c>
       <c r="B21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>175</v>
       </c>
       <c r="B22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>181</v>
       </c>
       <c r="B23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>182</v>
       </c>
       <c r="B24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>185</v>
       </c>
       <c r="B25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>186</v>
       </c>
       <c r="B26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>190</v>
       </c>
       <c r="B27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>248</v>
       </c>
       <c r="B28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>265</v>
       </c>
       <c r="B32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>70</v>
       </c>
       <c r="B33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>135</v>
       </c>
       <c r="B35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>155</v>
       </c>
       <c r="B36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>284</v>
       </c>
       <c r="B37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>176</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -15386,10 +15848,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F6FF9F-8B9B-488C-B485-3ABBC4416DFF}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" zoomScale="146" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15401,7 +15863,7 @@
     <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -15426,8 +15888,11 @@
       <c r="H1" s="13" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="20" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -15456,8 +15921,11 @@
         <f>0.0000000967</f>
         <v>9.6699999999999999E-8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -15486,8 +15954,11 @@
         <f>0.0000000119</f>
         <v>1.1900000000000001E-8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>295</v>
       </c>
@@ -15516,8 +15987,11 @@
         <f>0.00000012</f>
         <v>1.1999999999999999E-7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>296</v>
       </c>
@@ -15546,8 +16020,11 @@
         <f>0.000000301</f>
         <v>3.0100000000000001E-7</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>297</v>
       </c>
@@ -15576,8 +16053,11 @@
         <f>-0.000000103</f>
         <v>-1.03E-7</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>298</v>
       </c>
@@ -15605,8 +16085,11 @@
         <f>0.0000000356</f>
         <v>3.5600000000000001E-8</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>299</v>
       </c>
@@ -15635,8 +16118,11 @@
         <f>0.000000146</f>
         <v>1.4600000000000001E-7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>300</v>
       </c>
@@ -15665,8 +16151,11 @@
         <f>-0.0000000502</f>
         <v>-5.02E-8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>301</v>
       </c>
@@ -15694,8 +16183,11 @@
         <f>-0.000000018</f>
         <v>-1.7999999999999999E-8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>302</v>
       </c>
@@ -15724,8 +16216,11 @@
         <f>0.0000000624</f>
         <v>6.2400000000000003E-8</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>303</v>
       </c>
@@ -15754,8 +16249,11 @@
         <f>0.000000469</f>
         <v>4.6899999999999998E-7</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>304</v>
       </c>
@@ -15784,8 +16282,11 @@
         <f>-0.0000000159</f>
         <v>-1.59E-8</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>305</v>
       </c>
@@ -15814,8 +16315,11 @@
         <f>0.0000000678</f>
         <v>6.7799999999999998E-8</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>306</v>
       </c>
@@ -15843,8 +16347,11 @@
         <f>-0.0000000745</f>
         <v>-7.4499999999999999E-8</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>307</v>
       </c>
@@ -15873,8 +16380,11 @@
         <f>-0.0000000988</f>
         <v>-9.8799999999999998E-8</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>308</v>
       </c>
@@ -15903,8 +16413,11 @@
         <f>0.0000000494</f>
         <v>4.9399999999999999E-8</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>309</v>
       </c>
@@ -15933,8 +16446,11 @@
         <f>-0.0000000548</f>
         <v>-5.4800000000000001E-8</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>310</v>
       </c>
@@ -15963,8 +16479,11 @@
         <f>-0.0000000386</f>
         <v>-3.8600000000000002E-8</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>311</v>
       </c>
@@ -15992,8 +16511,11 @@
         <f>0.00000000286</f>
         <v>2.86E-9</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>312</v>
       </c>
@@ -16022,8 +16544,11 @@
         <f>-0.000000013</f>
         <v>-1.3000000000000001E-8</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>313</v>
       </c>
@@ -16052,8 +16577,11 @@
         <f>-0.0000000988</f>
         <v>-9.8799999999999998E-8</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -16082,8 +16610,11 @@
         <f>-0.0000000687</f>
         <v>-6.87E-8</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>314</v>
       </c>
@@ -16112,8 +16643,11 @@
         <f>-0.0000000452</f>
         <v>-4.5200000000000001E-8</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>315</v>
       </c>
@@ -16142,8 +16676,11 @@
         <f>-0.0000000178</f>
         <v>-1.7800000000000001E-8</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>316</v>
       </c>
@@ -16172,8 +16709,11 @@
         <f>-0.0000000976</f>
         <v>-9.76E-8</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -16201,8 +16741,11 @@
         <f>0.0000000105</f>
         <v>1.05E-8</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>317</v>
       </c>
@@ -16231,8 +16774,11 @@
         <f>-0.0000000628</f>
         <v>-6.2800000000000006E-8</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>318</v>
       </c>
@@ -16261,8 +16807,11 @@
         <f>0.000000146</f>
         <v>1.4600000000000001E-7</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>319</v>
       </c>
@@ -16287,8 +16836,11 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>320</v>
       </c>
@@ -16317,8 +16869,11 @@
         <f>-0.000000026</f>
         <v>-2.6000000000000001E-8</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>321</v>
       </c>
@@ -16347,8 +16902,11 @@
         <f>-0.0000000888</f>
         <v>-8.8800000000000001E-8</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>322</v>
       </c>
@@ -16377,8 +16935,11 @@
         <f>-0.0000000888</f>
         <v>-8.8800000000000001E-8</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>323</v>
       </c>
@@ -16406,6 +16967,9 @@
       <c r="H34">
         <f>-0.0000000211</f>
         <v>-2.11E-8</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -16473,7 +17037,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B3">
         <v>1.1378999999999999</v>
@@ -16519,7 +17083,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
@@ -16548,7 +17112,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B6" s="16">
         <f>LN(B5)*244.7889</f>
@@ -16565,7 +17129,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E7" s="16">
         <f>SQRT((4*(D5-15.7)^2+(E5-5.2)^2+(F5-5.8)^2))/3.3</f>

</xml_diff>

<commit_message>
added cyclic bonding constraint
</commit_message>
<xml_diff>
--- a/GCs.xlsx
+++ b/GCs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natur\Documents\AOBaddies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/att22_ic_ac_uk/Documents/AAYEAR4/APO1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD5CF5-EB09-40CD-A08F-45EA97C83165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="911" documentId="8_{1BB338DD-5CE3-4F3B-820B-FA7D83DA8823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4AA674E-550E-4557-9964-5AFB455E8856}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{8EFD0542-B832-47AD-A0F7-47D90D0B881B}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="338">
   <si>
     <t>Group</t>
   </si>
@@ -2903,9 +2903,6 @@
     <t>D0i</t>
   </si>
   <si>
-    <t>maxgroups</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
@@ -2916,6 +2913,12 @@
   </si>
   <si>
     <t>RED</t>
+  </si>
+  <si>
+    <t>nimax</t>
+  </si>
+  <si>
+    <t>nimin</t>
   </si>
   <si>
     <t>ai</t>
@@ -12515,10 +12518,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297960EB-DBC8-44A4-9F73-359D156C6248}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView zoomScale="71" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12526,7 +12529,7 @@
     <col min="4" max="4" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>227</v>
       </c>
@@ -12560,8 +12563,14 @@
       <c r="K1" s="13" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12595,8 +12604,14 @@
       <c r="K2">
         <v>2.3800000000000002E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12630,8 +12645,14 @@
       <c r="K3">
         <v>1.66E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12665,8 +12686,14 @@
       <c r="K4">
         <v>8.3999999999999995E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12700,8 +12727,14 @@
       <c r="K5">
         <v>-1.5E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -12735,8 +12768,14 @@
       <c r="K6">
         <v>1.2E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>19</v>
       </c>
@@ -12770,8 +12809,14 @@
       <c r="K7">
         <v>5.1999999999999998E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>8</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20</v>
       </c>
@@ -12805,8 +12850,14 @@
       <c r="K8">
         <v>3.0200000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>29</v>
       </c>
@@ -12840,8 +12891,14 @@
       <c r="K9">
         <v>4.1999999999999997E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>49</v>
       </c>
@@ -12875,8 +12932,14 @@
       <c r="K10">
         <v>2.81E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>50</v>
       </c>
@@ -12910,8 +12973,14 @@
       <c r="K11">
         <v>2.2800000000000001E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>54</v>
       </c>
@@ -12945,8 +13014,14 @@
       <c r="K12">
         <v>2.6200000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -12980,8 +13055,14 @@
       <c r="K13">
         <v>2.1399999999999999E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>57</v>
       </c>
@@ -13015,8 +13096,14 @@
       <c r="K14">
         <v>2.7900000000000001E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>58</v>
       </c>
@@ -13050,8 +13137,14 @@
       <c r="K15">
         <v>2.46E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>8</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>59</v>
       </c>
@@ -13085,8 +13178,14 @@
       <c r="K16">
         <v>1.8200000000000001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>60</v>
       </c>
@@ -13120,8 +13219,14 @@
       <c r="K17">
         <v>2.6499999999999999E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>61</v>
       </c>
@@ -13155,8 +13260,14 @@
       <c r="K18">
         <v>1.9E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>8</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>65</v>
       </c>
@@ -13190,8 +13301,14 @@
       <c r="K19">
         <v>9.5999999999999992E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>134</v>
       </c>
@@ -13225,8 +13342,14 @@
       <c r="K20">
         <v>4.1700000000000001E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>8</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>168</v>
       </c>
@@ -13260,8 +13383,14 @@
       <c r="K21">
         <v>1.6E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>8</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>169</v>
       </c>
@@ -13295,8 +13424,14 @@
       <c r="K22">
         <v>5.8999999999999999E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>8</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>175</v>
       </c>
@@ -13330,8 +13465,14 @@
       <c r="K23">
         <v>3.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>8</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>176</v>
       </c>
@@ -13365,8 +13506,14 @@
       <c r="K24">
         <v>1.6999999999999999E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>8</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>179</v>
       </c>
@@ -13400,8 +13547,14 @@
       <c r="K25">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>8</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>180</v>
       </c>
@@ -13435,8 +13588,14 @@
       <c r="K26">
         <v>1.2E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>8</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>184</v>
       </c>
@@ -13470,8 +13629,14 @@
       <c r="K27">
         <v>1.04E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>8</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>21</v>
       </c>
@@ -13505,8 +13670,14 @@
       <c r="K28" s="14">
         <v>2.29E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>8</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>30</v>
       </c>
@@ -13540,8 +13711,14 @@
       <c r="K29" s="14">
         <v>1.7000000000000001E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>8</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>31</v>
       </c>
@@ -13575,8 +13752,14 @@
       <c r="K30" s="14">
         <v>2.07E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>8</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>32</v>
       </c>
@@ -13610,8 +13793,14 @@
       <c r="K31" s="14">
         <v>4.7800000000000002E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>8</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>62</v>
       </c>
@@ -13645,8 +13834,14 @@
       <c r="K32" s="14">
         <v>2.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>8</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>63</v>
       </c>
@@ -13680,8 +13875,14 @@
       <c r="K33" s="14">
         <v>1.18E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>8</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>126</v>
       </c>
@@ -13715,8 +13916,14 @@
       <c r="K34" s="14">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>8</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>128</v>
       </c>
@@ -13750,8 +13957,14 @@
       <c r="K35" s="14">
         <v>2.1299999999999999E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>148</v>
       </c>
@@ -13785,8 +13998,14 @@
       <c r="K36" s="14">
         <v>1.43E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>8</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>149</v>
       </c>
@@ -13820,8 +14039,14 @@
       <c r="K37" s="14">
         <v>2.3699999999999999E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <v>8</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>170</v>
       </c>
@@ -13854,6 +14079,12 @@
       </c>
       <c r="K38" s="14">
         <v>0.13930000000000001</v>
+      </c>
+      <c r="L38">
+        <v>8</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -15070,10 +15301,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7EBF146-937E-4601-B58E-56AADBC56C60}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15081,308 +15312,533 @@
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>291</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="C1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>237</v>
       </c>
       <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>239</v>
       </c>
       <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>247</v>
       </c>
       <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
       <c r="B9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>257</v>
       </c>
       <c r="B10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>258</v>
       </c>
       <c r="B11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>259</v>
       </c>
       <c r="B12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>260</v>
       </c>
       <c r="B13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>261</v>
       </c>
       <c r="B14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>262</v>
       </c>
       <c r="B15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
       <c r="B16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>263</v>
       </c>
       <c r="B17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>264</v>
       </c>
       <c r="B18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>266</v>
       </c>
       <c r="B19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>278</v>
       </c>
       <c r="B20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>288</v>
       </c>
       <c r="B21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>175</v>
       </c>
       <c r="B22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>181</v>
       </c>
       <c r="B23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>182</v>
       </c>
       <c r="B24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>185</v>
       </c>
       <c r="B25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>186</v>
       </c>
       <c r="B26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>190</v>
       </c>
       <c r="B27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>248</v>
       </c>
       <c r="B28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>265</v>
       </c>
       <c r="B32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>70</v>
       </c>
       <c r="B33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>133</v>
       </c>
       <c r="B34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>135</v>
       </c>
       <c r="B35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>155</v>
       </c>
       <c r="B36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>284</v>
       </c>
       <c r="B37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>176</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -15394,7 +15850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F6FF9F-8B9B-488C-B485-3ABBC4416DFF}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="146" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
@@ -15433,7 +15889,7 @@
         <v>330</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -16581,7 +17037,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B3">
         <v>1.1378999999999999</v>
@@ -16627,7 +17083,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
@@ -16656,7 +17112,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B6" s="16">
         <f>LN(B5)*244.7889</f>
@@ -16673,7 +17129,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E7" s="16">
         <f>SQRT((4*(D5-15.7)^2+(E5-5.2)^2+(F5-5.8)^2))/3.3</f>

</xml_diff>

<commit_message>
fixed cyclic, solver is baron
</commit_message>
<xml_diff>
--- a/GCs.xlsx
+++ b/GCs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/att22_ic_ac_uk/Documents/AAYEAR4/APO1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natur\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="911" documentId="8_{1BB338DD-5CE3-4F3B-820B-FA7D83DA8823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4AA674E-550E-4557-9964-5AFB455E8856}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D0FEC2-8D4D-4328-B19E-4FDA916DFD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{8EFD0542-B832-47AD-A0F7-47D90D0B881B}"/>
+    <workbookView xWindow="31815" yWindow="2940" windowWidth="21600" windowHeight="10920" activeTab="2" xr2:uid="{8EFD0542-B832-47AD-A0F7-47D90D0B881B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3148,6 +3148,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3155,9 +3158,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -7469,16 +7469,16 @@
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A150" s="17">
+      <c r="A150" s="18">
         <v>149</v>
       </c>
-      <c r="B150" s="17" t="e" vm="1">
+      <c r="B150" s="18" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C150" s="17">
+      <c r="C150" s="18">
         <v>5.0639000000000003</v>
       </c>
-      <c r="D150" s="17">
+      <c r="D150" s="18">
         <v>6.4215</v>
       </c>
       <c r="E150" s="3">
@@ -7490,19 +7490,19 @@
       <c r="G150" s="3">
         <v>-0.33250000000000002</v>
       </c>
-      <c r="H150" s="17">
+      <c r="H150" s="18">
         <v>2.3699999999999999E-2</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A151" s="17"/>
-      <c r="B151" s="17"/>
-      <c r="C151" s="17"/>
-      <c r="D151" s="17"/>
+      <c r="A151" s="18"/>
+      <c r="B151" s="18"/>
+      <c r="C151" s="18"/>
+      <c r="D151" s="18"/>
       <c r="E151" s="3"/>
       <c r="F151" s="3"/>
       <c r="G151" s="3"/>
-      <c r="H151" s="17"/>
+      <c r="H151" s="18"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
@@ -12520,8 +12520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{297960EB-DBC8-44A4-9F73-359D156C6248}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView zoomScale="71" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13958,7 +13958,7 @@
         <v>2.1299999999999999E-2</v>
       </c>
       <c r="L35">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -15033,12 +15033,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -15850,8 +15850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F6FF9F-8B9B-488C-B485-3ABBC4416DFF}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="146" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15888,7 +15888,7 @@
       <c r="H1" s="13" t="s">
         <v>330</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>337</v>
       </c>
     </row>

</xml_diff>